<commit_message>
The commands in, dowJonesGraph.py are now called in mainWindow.py
</commit_message>
<xml_diff>
--- a/stock_dates_data.xlsx
+++ b/stock_dates_data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H97"/>
+  <dimension ref="B1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,22 +429,22 @@
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="2">
-        <v>43572</v>
+        <v>43577</v>
       </c>
       <c r="C2">
-        <v>26449.5</v>
+        <v>26511.1</v>
       </c>
       <c r="D2">
-        <v>26449.5</v>
+        <v>26511.1</v>
       </c>
       <c r="E2">
-        <v>26449.5</v>
+        <v>26511.1</v>
       </c>
       <c r="F2">
-        <v>26449.5</v>
+        <v>26511.1</v>
       </c>
       <c r="G2">
-        <v>26449.5</v>
+        <v>26511.1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -452,22 +452,22 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="2">
-        <v>43573</v>
+        <v>43578</v>
       </c>
       <c r="C3">
-        <v>26559.5</v>
+        <v>26656.4</v>
       </c>
       <c r="D3">
-        <v>26559.5</v>
+        <v>26656.4</v>
       </c>
       <c r="E3">
-        <v>26559.5</v>
+        <v>26656.4</v>
       </c>
       <c r="F3">
-        <v>26559.5</v>
+        <v>26656.4</v>
       </c>
       <c r="G3">
-        <v>26559.5</v>
+        <v>26656.4</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -475,22 +475,22 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="2">
-        <v>43577</v>
+        <v>43579</v>
       </c>
       <c r="C4">
-        <v>26511.1</v>
+        <v>26597</v>
       </c>
       <c r="D4">
-        <v>26511.1</v>
+        <v>26597</v>
       </c>
       <c r="E4">
-        <v>26511.1</v>
+        <v>26597</v>
       </c>
       <c r="F4">
-        <v>26511.1</v>
+        <v>26597</v>
       </c>
       <c r="G4">
-        <v>26511.1</v>
+        <v>26597</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -498,22 +498,22 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" s="2">
-        <v>43578</v>
+        <v>43580</v>
       </c>
       <c r="C5">
-        <v>26656.4</v>
+        <v>26462.1</v>
       </c>
       <c r="D5">
-        <v>26656.4</v>
+        <v>26462.1</v>
       </c>
       <c r="E5">
-        <v>26656.4</v>
+        <v>26462.1</v>
       </c>
       <c r="F5">
-        <v>26656.4</v>
+        <v>26462.1</v>
       </c>
       <c r="G5">
-        <v>26656.4</v>
+        <v>26462.1</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -521,22 +521,22 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="2">
-        <v>43579</v>
+        <v>43581</v>
       </c>
       <c r="C6">
-        <v>26597</v>
+        <v>26543.3</v>
       </c>
       <c r="D6">
-        <v>26597</v>
+        <v>26543.3</v>
       </c>
       <c r="E6">
-        <v>26597</v>
+        <v>26543.3</v>
       </c>
       <c r="F6">
-        <v>26597</v>
+        <v>26543.3</v>
       </c>
       <c r="G6">
-        <v>26597</v>
+        <v>26543.3</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -544,22 +544,22 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="2">
-        <v>43580</v>
+        <v>43584</v>
       </c>
       <c r="C7">
-        <v>26462.1</v>
+        <v>26554.4</v>
       </c>
       <c r="D7">
-        <v>26462.1</v>
+        <v>26554.4</v>
       </c>
       <c r="E7">
-        <v>26462.1</v>
+        <v>26554.4</v>
       </c>
       <c r="F7">
-        <v>26462.1</v>
+        <v>26554.4</v>
       </c>
       <c r="G7">
-        <v>26462.1</v>
+        <v>26554.4</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -567,22 +567,22 @@
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="2">
-        <v>43581</v>
+        <v>43585</v>
       </c>
       <c r="C8">
-        <v>26543.3</v>
+        <v>26592.9</v>
       </c>
       <c r="D8">
-        <v>26543.3</v>
+        <v>26592.9</v>
       </c>
       <c r="E8">
-        <v>26543.3</v>
+        <v>26592.9</v>
       </c>
       <c r="F8">
-        <v>26543.3</v>
+        <v>26592.9</v>
       </c>
       <c r="G8">
-        <v>26543.3</v>
+        <v>26592.9</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -590,22 +590,22 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="2">
-        <v>43584</v>
+        <v>43586</v>
       </c>
       <c r="C9">
-        <v>26554.4</v>
+        <v>26430.1</v>
       </c>
       <c r="D9">
-        <v>26554.4</v>
+        <v>26430.1</v>
       </c>
       <c r="E9">
-        <v>26554.4</v>
+        <v>26430.1</v>
       </c>
       <c r="F9">
-        <v>26554.4</v>
+        <v>26430.1</v>
       </c>
       <c r="G9">
-        <v>26554.4</v>
+        <v>26430.1</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -613,22 +613,22 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="2">
-        <v>43585</v>
+        <v>43588</v>
       </c>
       <c r="C10">
-        <v>26592.9</v>
+        <v>26504.9</v>
       </c>
       <c r="D10">
-        <v>26592.9</v>
+        <v>26504.9</v>
       </c>
       <c r="E10">
-        <v>26592.9</v>
+        <v>26504.9</v>
       </c>
       <c r="F10">
-        <v>26592.9</v>
+        <v>26504.9</v>
       </c>
       <c r="G10">
-        <v>26592.9</v>
+        <v>26504.9</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -636,22 +636,22 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="2">
-        <v>43586</v>
+        <v>43591</v>
       </c>
       <c r="C11">
-        <v>26430.1</v>
+        <v>26438.5</v>
       </c>
       <c r="D11">
-        <v>26430.1</v>
+        <v>26438.5</v>
       </c>
       <c r="E11">
-        <v>26430.1</v>
+        <v>26438.5</v>
       </c>
       <c r="F11">
-        <v>26430.1</v>
+        <v>26438.5</v>
       </c>
       <c r="G11">
-        <v>26430.1</v>
+        <v>26438.5</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -659,22 +659,22 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="2">
-        <v>43588</v>
+        <v>43592</v>
       </c>
       <c r="C12">
-        <v>26504.9</v>
+        <v>25965.1</v>
       </c>
       <c r="D12">
-        <v>26504.9</v>
+        <v>25965.1</v>
       </c>
       <c r="E12">
-        <v>26504.9</v>
+        <v>25965.1</v>
       </c>
       <c r="F12">
-        <v>26504.9</v>
+        <v>25965.1</v>
       </c>
       <c r="G12">
-        <v>26504.9</v>
+        <v>25965.1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -682,22 +682,22 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="2">
-        <v>43591</v>
+        <v>43593</v>
       </c>
       <c r="C13">
-        <v>26438.5</v>
+        <v>25967.3</v>
       </c>
       <c r="D13">
-        <v>26438.5</v>
+        <v>25967.3</v>
       </c>
       <c r="E13">
-        <v>26438.5</v>
+        <v>25967.3</v>
       </c>
       <c r="F13">
-        <v>26438.5</v>
+        <v>25967.3</v>
       </c>
       <c r="G13">
-        <v>26438.5</v>
+        <v>25967.3</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -705,22 +705,22 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="2">
-        <v>43592</v>
+        <v>43594</v>
       </c>
       <c r="C14">
-        <v>25965.1</v>
+        <v>25828.4</v>
       </c>
       <c r="D14">
-        <v>25965.1</v>
+        <v>25828.4</v>
       </c>
       <c r="E14">
-        <v>25965.1</v>
+        <v>25828.4</v>
       </c>
       <c r="F14">
-        <v>25965.1</v>
+        <v>25828.4</v>
       </c>
       <c r="G14">
-        <v>25965.1</v>
+        <v>25828.4</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -728,22 +728,22 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="2">
-        <v>43593</v>
+        <v>43595</v>
       </c>
       <c r="C15">
-        <v>25967.3</v>
+        <v>25942.4</v>
       </c>
       <c r="D15">
-        <v>25967.3</v>
+        <v>25942.4</v>
       </c>
       <c r="E15">
-        <v>25967.3</v>
+        <v>25942.4</v>
       </c>
       <c r="F15">
-        <v>25967.3</v>
+        <v>25942.4</v>
       </c>
       <c r="G15">
-        <v>25967.3</v>
+        <v>25942.4</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -751,22 +751,22 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="2">
-        <v>43594</v>
+        <v>43598</v>
       </c>
       <c r="C16">
-        <v>25828.4</v>
+        <v>25325</v>
       </c>
       <c r="D16">
-        <v>25828.4</v>
+        <v>25325</v>
       </c>
       <c r="E16">
-        <v>25828.4</v>
+        <v>25325</v>
       </c>
       <c r="F16">
-        <v>25828.4</v>
+        <v>25325</v>
       </c>
       <c r="G16">
-        <v>25828.4</v>
+        <v>25325</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -774,22 +774,22 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="2">
-        <v>43595</v>
+        <v>43599</v>
       </c>
       <c r="C17">
-        <v>25942.4</v>
+        <v>25532</v>
       </c>
       <c r="D17">
-        <v>25942.4</v>
+        <v>25532</v>
       </c>
       <c r="E17">
-        <v>25942.4</v>
+        <v>25532</v>
       </c>
       <c r="F17">
-        <v>25942.4</v>
+        <v>25532</v>
       </c>
       <c r="G17">
-        <v>25942.4</v>
+        <v>25532</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -797,22 +797,22 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="2">
-        <v>43598</v>
+        <v>43600</v>
       </c>
       <c r="C18">
-        <v>25325</v>
+        <v>25648</v>
       </c>
       <c r="D18">
-        <v>25325</v>
+        <v>25648</v>
       </c>
       <c r="E18">
-        <v>25325</v>
+        <v>25648</v>
       </c>
       <c r="F18">
-        <v>25325</v>
+        <v>25648</v>
       </c>
       <c r="G18">
-        <v>25325</v>
+        <v>25648</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -820,22 +820,22 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="2">
-        <v>43599</v>
+        <v>43601</v>
       </c>
       <c r="C19">
-        <v>25532</v>
+        <v>25862.7</v>
       </c>
       <c r="D19">
-        <v>25532</v>
+        <v>25862.7</v>
       </c>
       <c r="E19">
-        <v>25532</v>
+        <v>25862.7</v>
       </c>
       <c r="F19">
-        <v>25532</v>
+        <v>25862.7</v>
       </c>
       <c r="G19">
-        <v>25532</v>
+        <v>25862.7</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -843,22 +843,22 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="2">
-        <v>43600</v>
+        <v>43602</v>
       </c>
       <c r="C20">
-        <v>25648</v>
+        <v>25764</v>
       </c>
       <c r="D20">
-        <v>25648</v>
+        <v>25764</v>
       </c>
       <c r="E20">
-        <v>25648</v>
+        <v>25764</v>
       </c>
       <c r="F20">
-        <v>25648</v>
+        <v>25764</v>
       </c>
       <c r="G20">
-        <v>25648</v>
+        <v>25764</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -866,22 +866,22 @@
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="2">
-        <v>43601</v>
+        <v>43605</v>
       </c>
       <c r="C21">
-        <v>25862.7</v>
+        <v>25679.9</v>
       </c>
       <c r="D21">
-        <v>25862.7</v>
+        <v>25679.9</v>
       </c>
       <c r="E21">
-        <v>25862.7</v>
+        <v>25679.9</v>
       </c>
       <c r="F21">
-        <v>25862.7</v>
+        <v>25679.9</v>
       </c>
       <c r="G21">
-        <v>25862.7</v>
+        <v>25679.9</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -889,22 +889,22 @@
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="2">
-        <v>43602</v>
+        <v>43606</v>
       </c>
       <c r="C22">
-        <v>25764</v>
+        <v>25877.3</v>
       </c>
       <c r="D22">
-        <v>25764</v>
+        <v>25877.3</v>
       </c>
       <c r="E22">
-        <v>25764</v>
+        <v>25877.3</v>
       </c>
       <c r="F22">
-        <v>25764</v>
+        <v>25877.3</v>
       </c>
       <c r="G22">
-        <v>25764</v>
+        <v>25877.3</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -912,22 +912,22 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="2">
-        <v>43605</v>
+        <v>43607</v>
       </c>
       <c r="C23">
-        <v>25679.9</v>
+        <v>25776.6</v>
       </c>
       <c r="D23">
-        <v>25679.9</v>
+        <v>25776.6</v>
       </c>
       <c r="E23">
-        <v>25679.9</v>
+        <v>25776.6</v>
       </c>
       <c r="F23">
-        <v>25679.9</v>
+        <v>25776.6</v>
       </c>
       <c r="G23">
-        <v>25679.9</v>
+        <v>25776.6</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -935,22 +935,22 @@
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="2">
-        <v>43606</v>
+        <v>43608</v>
       </c>
       <c r="C24">
-        <v>25877.3</v>
+        <v>25490.5</v>
       </c>
       <c r="D24">
-        <v>25877.3</v>
+        <v>25490.5</v>
       </c>
       <c r="E24">
-        <v>25877.3</v>
+        <v>25490.5</v>
       </c>
       <c r="F24">
-        <v>25877.3</v>
+        <v>25490.5</v>
       </c>
       <c r="G24">
-        <v>25877.3</v>
+        <v>25490.5</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -958,22 +958,22 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="2">
-        <v>43607</v>
+        <v>43609</v>
       </c>
       <c r="C25">
-        <v>25776.6</v>
+        <v>25585.7</v>
       </c>
       <c r="D25">
-        <v>25776.6</v>
+        <v>25585.7</v>
       </c>
       <c r="E25">
-        <v>25776.6</v>
+        <v>25585.7</v>
       </c>
       <c r="F25">
-        <v>25776.6</v>
+        <v>25585.7</v>
       </c>
       <c r="G25">
-        <v>25776.6</v>
+        <v>25585.7</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -981,22 +981,22 @@
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="2">
-        <v>43608</v>
+        <v>43613</v>
       </c>
       <c r="C26">
-        <v>25490.5</v>
+        <v>25347.8</v>
       </c>
       <c r="D26">
-        <v>25490.5</v>
+        <v>25347.8</v>
       </c>
       <c r="E26">
-        <v>25490.5</v>
+        <v>25347.8</v>
       </c>
       <c r="F26">
-        <v>25490.5</v>
+        <v>25347.8</v>
       </c>
       <c r="G26">
-        <v>25490.5</v>
+        <v>25347.8</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1004,22 +1004,22 @@
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="2">
-        <v>43609</v>
+        <v>43614</v>
       </c>
       <c r="C27">
-        <v>25585.7</v>
+        <v>25126.4</v>
       </c>
       <c r="D27">
-        <v>25585.7</v>
+        <v>25126.4</v>
       </c>
       <c r="E27">
-        <v>25585.7</v>
+        <v>25126.4</v>
       </c>
       <c r="F27">
-        <v>25585.7</v>
+        <v>25126.4</v>
       </c>
       <c r="G27">
-        <v>25585.7</v>
+        <v>25126.4</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1027,22 +1027,22 @@
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="2">
-        <v>43613</v>
+        <v>43615</v>
       </c>
       <c r="C28">
-        <v>25347.8</v>
+        <v>25169.9</v>
       </c>
       <c r="D28">
-        <v>25347.8</v>
+        <v>25169.9</v>
       </c>
       <c r="E28">
-        <v>25347.8</v>
+        <v>25169.9</v>
       </c>
       <c r="F28">
-        <v>25347.8</v>
+        <v>25169.9</v>
       </c>
       <c r="G28">
-        <v>25347.8</v>
+        <v>25169.9</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1050,22 +1050,22 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="2">
-        <v>43614</v>
+        <v>43616</v>
       </c>
       <c r="C29">
-        <v>25126.4</v>
+        <v>24815</v>
       </c>
       <c r="D29">
-        <v>25126.4</v>
+        <v>24815</v>
       </c>
       <c r="E29">
-        <v>25126.4</v>
+        <v>24815</v>
       </c>
       <c r="F29">
-        <v>25126.4</v>
+        <v>24815</v>
       </c>
       <c r="G29">
-        <v>25126.4</v>
+        <v>24815</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1073,22 +1073,22 @@
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="2">
-        <v>43615</v>
+        <v>43619</v>
       </c>
       <c r="C30">
-        <v>25169.9</v>
+        <v>24819.8</v>
       </c>
       <c r="D30">
-        <v>25169.9</v>
+        <v>24819.8</v>
       </c>
       <c r="E30">
-        <v>25169.9</v>
+        <v>24819.8</v>
       </c>
       <c r="F30">
-        <v>25169.9</v>
+        <v>24819.8</v>
       </c>
       <c r="G30">
-        <v>25169.9</v>
+        <v>24819.8</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1096,22 +1096,22 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="2">
-        <v>43616</v>
+        <v>43620</v>
       </c>
       <c r="C31">
-        <v>24815</v>
+        <v>25332.2</v>
       </c>
       <c r="D31">
-        <v>24815</v>
+        <v>25332.2</v>
       </c>
       <c r="E31">
-        <v>24815</v>
+        <v>25332.2</v>
       </c>
       <c r="F31">
-        <v>24815</v>
+        <v>25332.2</v>
       </c>
       <c r="G31">
-        <v>24815</v>
+        <v>25332.2</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1119,22 +1119,22 @@
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="2">
-        <v>43619</v>
+        <v>43621</v>
       </c>
       <c r="C32">
-        <v>24819.8</v>
+        <v>25539.6</v>
       </c>
       <c r="D32">
-        <v>24819.8</v>
+        <v>25539.6</v>
       </c>
       <c r="E32">
-        <v>24819.8</v>
+        <v>25539.6</v>
       </c>
       <c r="F32">
-        <v>24819.8</v>
+        <v>25539.6</v>
       </c>
       <c r="G32">
-        <v>24819.8</v>
+        <v>25539.6</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1142,22 +1142,22 @@
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="2">
-        <v>43620</v>
+        <v>43623</v>
       </c>
       <c r="C33">
-        <v>25332.2</v>
+        <v>25983.9</v>
       </c>
       <c r="D33">
-        <v>25332.2</v>
+        <v>25983.9</v>
       </c>
       <c r="E33">
-        <v>25332.2</v>
+        <v>25983.9</v>
       </c>
       <c r="F33">
-        <v>25332.2</v>
+        <v>25983.9</v>
       </c>
       <c r="G33">
-        <v>25332.2</v>
+        <v>25983.9</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1165,22 +1165,22 @@
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="2">
-        <v>43621</v>
+        <v>43636</v>
       </c>
       <c r="C34">
-        <v>25539.6</v>
+        <v>26753.2</v>
       </c>
       <c r="D34">
-        <v>25539.6</v>
+        <v>26753.2</v>
       </c>
       <c r="E34">
-        <v>25539.6</v>
+        <v>26753.2</v>
       </c>
       <c r="F34">
-        <v>25539.6</v>
+        <v>26753.2</v>
       </c>
       <c r="G34">
-        <v>25539.6</v>
+        <v>26753.2</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -1188,22 +1188,22 @@
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="2">
-        <v>43623</v>
+        <v>43735</v>
       </c>
       <c r="C35">
-        <v>25983.9</v>
+        <v>26820.2</v>
       </c>
       <c r="D35">
-        <v>25983.9</v>
+        <v>26820.2</v>
       </c>
       <c r="E35">
-        <v>25983.9</v>
+        <v>26820.2</v>
       </c>
       <c r="F35">
-        <v>25983.9</v>
+        <v>26820.2</v>
       </c>
       <c r="G35">
-        <v>25983.9</v>
+        <v>26820.2</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1211,22 +1211,22 @@
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="2">
-        <v>43636</v>
+        <v>43754</v>
       </c>
       <c r="C36">
-        <v>26753.2</v>
+        <v>27002</v>
       </c>
       <c r="D36">
-        <v>26753.2</v>
+        <v>27002</v>
       </c>
       <c r="E36">
-        <v>26753.2</v>
+        <v>27002</v>
       </c>
       <c r="F36">
-        <v>26753.2</v>
+        <v>27002</v>
       </c>
       <c r="G36">
-        <v>26753.2</v>
+        <v>27002</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1234,22 +1234,22 @@
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="2">
-        <v>43735</v>
+        <v>43853</v>
       </c>
       <c r="C37">
-        <v>26820.2</v>
+        <v>29160.1</v>
       </c>
       <c r="D37">
-        <v>26820.2</v>
+        <v>29160.1</v>
       </c>
       <c r="E37">
-        <v>26820.2</v>
+        <v>29160.1</v>
       </c>
       <c r="F37">
-        <v>26820.2</v>
+        <v>29160.1</v>
       </c>
       <c r="G37">
-        <v>26820.2</v>
+        <v>29160.1</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -1257,22 +1257,22 @@
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="2">
-        <v>43754</v>
+        <v>43854</v>
       </c>
       <c r="C38">
-        <v>27002</v>
+        <v>28989.7</v>
       </c>
       <c r="D38">
-        <v>27002</v>
+        <v>28989.7</v>
       </c>
       <c r="E38">
-        <v>27002</v>
+        <v>28989.7</v>
       </c>
       <c r="F38">
-        <v>27002</v>
+        <v>28989.7</v>
       </c>
       <c r="G38">
-        <v>27002</v>
+        <v>28989.7</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -1280,22 +1280,22 @@
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="2">
-        <v>43853</v>
+        <v>43857</v>
       </c>
       <c r="C39">
-        <v>29160.1</v>
+        <v>28535.8</v>
       </c>
       <c r="D39">
-        <v>29160.1</v>
+        <v>28535.8</v>
       </c>
       <c r="E39">
-        <v>29160.1</v>
+        <v>28535.8</v>
       </c>
       <c r="F39">
-        <v>29160.1</v>
+        <v>28535.8</v>
       </c>
       <c r="G39">
-        <v>29160.1</v>
+        <v>28535.8</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -1303,22 +1303,22 @@
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="2">
-        <v>43854</v>
+        <v>43858</v>
       </c>
       <c r="C40">
-        <v>28989.7</v>
+        <v>28722.8</v>
       </c>
       <c r="D40">
-        <v>28989.7</v>
+        <v>28722.8</v>
       </c>
       <c r="E40">
-        <v>28989.7</v>
+        <v>28722.8</v>
       </c>
       <c r="F40">
-        <v>28989.7</v>
+        <v>28722.8</v>
       </c>
       <c r="G40">
-        <v>28989.7</v>
+        <v>28722.8</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -1326,22 +1326,22 @@
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="2">
-        <v>43857</v>
+        <v>43859</v>
       </c>
       <c r="C41">
-        <v>28535.8</v>
+        <v>28734.4</v>
       </c>
       <c r="D41">
-        <v>28535.8</v>
+        <v>28734.4</v>
       </c>
       <c r="E41">
-        <v>28535.8</v>
+        <v>28734.4</v>
       </c>
       <c r="F41">
-        <v>28535.8</v>
+        <v>28734.4</v>
       </c>
       <c r="G41">
-        <v>28535.8</v>
+        <v>28734.4</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -1349,22 +1349,22 @@
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="2">
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="C42">
-        <v>28722.8</v>
+        <v>28859.4</v>
       </c>
       <c r="D42">
-        <v>28722.8</v>
+        <v>28859.4</v>
       </c>
       <c r="E42">
-        <v>28722.8</v>
+        <v>28859.4</v>
       </c>
       <c r="F42">
-        <v>28722.8</v>
+        <v>28859.4</v>
       </c>
       <c r="G42">
-        <v>28722.8</v>
+        <v>28859.4</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -1372,22 +1372,22 @@
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="2">
-        <v>43859</v>
+        <v>43861</v>
       </c>
       <c r="C43">
-        <v>28734.4</v>
+        <v>28256</v>
       </c>
       <c r="D43">
-        <v>28734.4</v>
+        <v>28256</v>
       </c>
       <c r="E43">
-        <v>28734.4</v>
+        <v>28256</v>
       </c>
       <c r="F43">
-        <v>28734.4</v>
+        <v>28256</v>
       </c>
       <c r="G43">
-        <v>28734.4</v>
+        <v>28256</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -1395,22 +1395,22 @@
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="2">
-        <v>43860</v>
+        <v>43864</v>
       </c>
       <c r="C44">
-        <v>28859.4</v>
+        <v>28399.8</v>
       </c>
       <c r="D44">
-        <v>28859.4</v>
+        <v>28399.8</v>
       </c>
       <c r="E44">
-        <v>28859.4</v>
+        <v>28399.8</v>
       </c>
       <c r="F44">
-        <v>28859.4</v>
+        <v>28399.8</v>
       </c>
       <c r="G44">
-        <v>28859.4</v>
+        <v>28399.8</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -1418,22 +1418,22 @@
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="2">
-        <v>43861</v>
+        <v>43865</v>
       </c>
       <c r="C45">
-        <v>28256</v>
+        <v>28807.6</v>
       </c>
       <c r="D45">
-        <v>28256</v>
+        <v>28807.6</v>
       </c>
       <c r="E45">
-        <v>28256</v>
+        <v>28807.6</v>
       </c>
       <c r="F45">
-        <v>28256</v>
+        <v>28807.6</v>
       </c>
       <c r="G45">
-        <v>28256</v>
+        <v>28807.6</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -1441,22 +1441,22 @@
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="2">
-        <v>43864</v>
+        <v>43866</v>
       </c>
       <c r="C46">
-        <v>28399.8</v>
+        <v>29290.9</v>
       </c>
       <c r="D46">
-        <v>28399.8</v>
+        <v>29290.9</v>
       </c>
       <c r="E46">
-        <v>28399.8</v>
+        <v>29290.9</v>
       </c>
       <c r="F46">
-        <v>28399.8</v>
+        <v>29290.9</v>
       </c>
       <c r="G46">
-        <v>28399.8</v>
+        <v>29290.9</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -1464,22 +1464,22 @@
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="2">
-        <v>43865</v>
+        <v>43867</v>
       </c>
       <c r="C47">
-        <v>28807.6</v>
+        <v>29379.8</v>
       </c>
       <c r="D47">
-        <v>28807.6</v>
+        <v>29379.8</v>
       </c>
       <c r="E47">
-        <v>28807.6</v>
+        <v>29379.8</v>
       </c>
       <c r="F47">
-        <v>28807.6</v>
+        <v>29379.8</v>
       </c>
       <c r="G47">
-        <v>28807.6</v>
+        <v>29379.8</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -1487,22 +1487,22 @@
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="2">
-        <v>43866</v>
+        <v>43868</v>
       </c>
       <c r="C48">
-        <v>29290.9</v>
+        <v>29102.5</v>
       </c>
       <c r="D48">
-        <v>29290.9</v>
+        <v>29102.5</v>
       </c>
       <c r="E48">
-        <v>29290.9</v>
+        <v>29102.5</v>
       </c>
       <c r="F48">
-        <v>29290.9</v>
+        <v>29102.5</v>
       </c>
       <c r="G48">
-        <v>29290.9</v>
+        <v>29102.5</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -1510,22 +1510,22 @@
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="2">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="C49">
-        <v>29379.8</v>
+        <v>29276.8</v>
       </c>
       <c r="D49">
-        <v>29379.8</v>
+        <v>29276.8</v>
       </c>
       <c r="E49">
-        <v>29379.8</v>
+        <v>29276.8</v>
       </c>
       <c r="F49">
-        <v>29379.8</v>
+        <v>29276.8</v>
       </c>
       <c r="G49">
-        <v>29379.8</v>
+        <v>29276.8</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -1533,22 +1533,22 @@
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="2">
-        <v>43868</v>
+        <v>43872</v>
       </c>
       <c r="C50">
-        <v>29102.5</v>
+        <v>29276.3</v>
       </c>
       <c r="D50">
-        <v>29102.5</v>
+        <v>29276.3</v>
       </c>
       <c r="E50">
-        <v>29102.5</v>
+        <v>29276.3</v>
       </c>
       <c r="F50">
-        <v>29102.5</v>
+        <v>29276.3</v>
       </c>
       <c r="G50">
-        <v>29102.5</v>
+        <v>29276.3</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -1556,22 +1556,22 @@
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="2">
-        <v>43871</v>
+        <v>43873</v>
       </c>
       <c r="C51">
-        <v>29276.8</v>
+        <v>29551.4</v>
       </c>
       <c r="D51">
-        <v>29276.8</v>
+        <v>29551.4</v>
       </c>
       <c r="E51">
-        <v>29276.8</v>
+        <v>29551.4</v>
       </c>
       <c r="F51">
-        <v>29276.8</v>
+        <v>29551.4</v>
       </c>
       <c r="G51">
-        <v>29276.8</v>
+        <v>29551.4</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -1579,22 +1579,22 @@
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="2">
-        <v>43872</v>
+        <v>43874</v>
       </c>
       <c r="C52">
-        <v>29276.3</v>
+        <v>29423.3</v>
       </c>
       <c r="D52">
-        <v>29276.3</v>
+        <v>29423.3</v>
       </c>
       <c r="E52">
-        <v>29276.3</v>
+        <v>29423.3</v>
       </c>
       <c r="F52">
-        <v>29276.3</v>
+        <v>29423.3</v>
       </c>
       <c r="G52">
-        <v>29276.3</v>
+        <v>29423.3</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -1602,22 +1602,22 @@
     </row>
     <row r="53" spans="2:8">
       <c r="B53" s="2">
-        <v>43873</v>
+        <v>43875</v>
       </c>
       <c r="C53">
-        <v>29551.4</v>
+        <v>29398.1</v>
       </c>
       <c r="D53">
-        <v>29551.4</v>
+        <v>29398.1</v>
       </c>
       <c r="E53">
-        <v>29551.4</v>
+        <v>29398.1</v>
       </c>
       <c r="F53">
-        <v>29551.4</v>
+        <v>29398.1</v>
       </c>
       <c r="G53">
-        <v>29551.4</v>
+        <v>29398.1</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -1625,22 +1625,22 @@
     </row>
     <row r="54" spans="2:8">
       <c r="B54" s="2">
-        <v>43874</v>
+        <v>43879</v>
       </c>
       <c r="C54">
-        <v>29423.3</v>
+        <v>29232.2</v>
       </c>
       <c r="D54">
-        <v>29423.3</v>
+        <v>29232.2</v>
       </c>
       <c r="E54">
-        <v>29423.3</v>
+        <v>29232.2</v>
       </c>
       <c r="F54">
-        <v>29423.3</v>
+        <v>29232.2</v>
       </c>
       <c r="G54">
-        <v>29423.3</v>
+        <v>29232.2</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -1648,22 +1648,22 @@
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="2">
-        <v>43875</v>
+        <v>43880</v>
       </c>
       <c r="C55">
-        <v>29398.1</v>
+        <v>29348</v>
       </c>
       <c r="D55">
-        <v>29398.1</v>
+        <v>29348</v>
       </c>
       <c r="E55">
-        <v>29398.1</v>
+        <v>29348</v>
       </c>
       <c r="F55">
-        <v>29398.1</v>
+        <v>29348</v>
       </c>
       <c r="G55">
-        <v>29398.1</v>
+        <v>29348</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -1671,22 +1671,22 @@
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="2">
-        <v>43879</v>
+        <v>43881</v>
       </c>
       <c r="C56">
-        <v>29232.2</v>
+        <v>29220</v>
       </c>
       <c r="D56">
-        <v>29232.2</v>
+        <v>29220</v>
       </c>
       <c r="E56">
-        <v>29232.2</v>
+        <v>29220</v>
       </c>
       <c r="F56">
-        <v>29232.2</v>
+        <v>29220</v>
       </c>
       <c r="G56">
-        <v>29232.2</v>
+        <v>29220</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -1694,22 +1694,22 @@
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="2">
-        <v>43880</v>
+        <v>43882</v>
       </c>
       <c r="C57">
-        <v>29348</v>
+        <v>28992.4</v>
       </c>
       <c r="D57">
-        <v>29348</v>
+        <v>28992.4</v>
       </c>
       <c r="E57">
-        <v>29348</v>
+        <v>28992.4</v>
       </c>
       <c r="F57">
-        <v>29348</v>
+        <v>28992.4</v>
       </c>
       <c r="G57">
-        <v>29348</v>
+        <v>28992.4</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -1717,22 +1717,22 @@
     </row>
     <row r="58" spans="2:8">
       <c r="B58" s="2">
-        <v>43881</v>
+        <v>43885</v>
       </c>
       <c r="C58">
-        <v>29220</v>
+        <v>27960.8</v>
       </c>
       <c r="D58">
-        <v>29220</v>
+        <v>27960.8</v>
       </c>
       <c r="E58">
-        <v>29220</v>
+        <v>27960.8</v>
       </c>
       <c r="F58">
-        <v>29220</v>
+        <v>27960.8</v>
       </c>
       <c r="G58">
-        <v>29220</v>
+        <v>27960.8</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -1740,22 +1740,22 @@
     </row>
     <row r="59" spans="2:8">
       <c r="B59" s="2">
-        <v>43882</v>
+        <v>43886</v>
       </c>
       <c r="C59">
-        <v>28992.4</v>
+        <v>27081.4</v>
       </c>
       <c r="D59">
-        <v>28992.4</v>
+        <v>27081.4</v>
       </c>
       <c r="E59">
-        <v>28992.4</v>
+        <v>27081.4</v>
       </c>
       <c r="F59">
-        <v>28992.4</v>
+        <v>27081.4</v>
       </c>
       <c r="G59">
-        <v>28992.4</v>
+        <v>27081.4</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -1763,22 +1763,22 @@
     </row>
     <row r="60" spans="2:8">
       <c r="B60" s="2">
-        <v>43885</v>
+        <v>43887</v>
       </c>
       <c r="C60">
-        <v>27960.8</v>
+        <v>26957.6</v>
       </c>
       <c r="D60">
-        <v>27960.8</v>
+        <v>26957.6</v>
       </c>
       <c r="E60">
-        <v>27960.8</v>
+        <v>26957.6</v>
       </c>
       <c r="F60">
-        <v>27960.8</v>
+        <v>26957.6</v>
       </c>
       <c r="G60">
-        <v>27960.8</v>
+        <v>26957.6</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -1786,22 +1786,22 @@
     </row>
     <row r="61" spans="2:8">
       <c r="B61" s="2">
-        <v>43886</v>
+        <v>43888</v>
       </c>
       <c r="C61">
-        <v>27081.4</v>
+        <v>25766.6</v>
       </c>
       <c r="D61">
-        <v>27081.4</v>
+        <v>25766.6</v>
       </c>
       <c r="E61">
-        <v>27081.4</v>
+        <v>25766.6</v>
       </c>
       <c r="F61">
-        <v>27081.4</v>
+        <v>25766.6</v>
       </c>
       <c r="G61">
-        <v>27081.4</v>
+        <v>25766.6</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -1809,22 +1809,22 @@
     </row>
     <row r="62" spans="2:8">
       <c r="B62" s="2">
-        <v>43887</v>
+        <v>43889</v>
       </c>
       <c r="C62">
-        <v>26957.6</v>
+        <v>25409.4</v>
       </c>
       <c r="D62">
-        <v>26957.6</v>
+        <v>25409.4</v>
       </c>
       <c r="E62">
-        <v>26957.6</v>
+        <v>25409.4</v>
       </c>
       <c r="F62">
-        <v>26957.6</v>
+        <v>25409.4</v>
       </c>
       <c r="G62">
-        <v>26957.6</v>
+        <v>25409.4</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -1832,22 +1832,22 @@
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="2">
-        <v>43888</v>
+        <v>43892</v>
       </c>
       <c r="C63">
-        <v>25766.6</v>
+        <v>26703.3</v>
       </c>
       <c r="D63">
-        <v>25766.6</v>
+        <v>26703.3</v>
       </c>
       <c r="E63">
-        <v>25766.6</v>
+        <v>26703.3</v>
       </c>
       <c r="F63">
-        <v>25766.6</v>
+        <v>26703.3</v>
       </c>
       <c r="G63">
-        <v>25766.6</v>
+        <v>26703.3</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -1855,22 +1855,22 @@
     </row>
     <row r="64" spans="2:8">
       <c r="B64" s="2">
-        <v>43889</v>
+        <v>43893</v>
       </c>
       <c r="C64">
-        <v>25409.4</v>
+        <v>25917.4</v>
       </c>
       <c r="D64">
-        <v>25409.4</v>
+        <v>25917.4</v>
       </c>
       <c r="E64">
-        <v>25409.4</v>
+        <v>25917.4</v>
       </c>
       <c r="F64">
-        <v>25409.4</v>
+        <v>25917.4</v>
       </c>
       <c r="G64">
-        <v>25409.4</v>
+        <v>25917.4</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -1878,22 +1878,22 @@
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="2">
-        <v>43892</v>
+        <v>43894</v>
       </c>
       <c r="C65">
-        <v>26703.3</v>
+        <v>27090.9</v>
       </c>
       <c r="D65">
-        <v>26703.3</v>
+        <v>27090.9</v>
       </c>
       <c r="E65">
-        <v>26703.3</v>
+        <v>27090.9</v>
       </c>
       <c r="F65">
-        <v>26703.3</v>
+        <v>27090.9</v>
       </c>
       <c r="G65">
-        <v>26703.3</v>
+        <v>27090.9</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -1901,22 +1901,22 @@
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="2">
-        <v>43893</v>
+        <v>43895</v>
       </c>
       <c r="C66">
-        <v>25917.4</v>
+        <v>26121.3</v>
       </c>
       <c r="D66">
-        <v>25917.4</v>
+        <v>26121.3</v>
       </c>
       <c r="E66">
-        <v>25917.4</v>
+        <v>26121.3</v>
       </c>
       <c r="F66">
-        <v>25917.4</v>
+        <v>26121.3</v>
       </c>
       <c r="G66">
-        <v>25917.4</v>
+        <v>26121.3</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -1924,22 +1924,22 @@
     </row>
     <row r="67" spans="2:8">
       <c r="B67" s="2">
-        <v>43894</v>
+        <v>43896</v>
       </c>
       <c r="C67">
-        <v>27090.9</v>
+        <v>25864.8</v>
       </c>
       <c r="D67">
-        <v>27090.9</v>
+        <v>25864.8</v>
       </c>
       <c r="E67">
-        <v>27090.9</v>
+        <v>25864.8</v>
       </c>
       <c r="F67">
-        <v>27090.9</v>
+        <v>25864.8</v>
       </c>
       <c r="G67">
-        <v>27090.9</v>
+        <v>25864.8</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -1947,22 +1947,22 @@
     </row>
     <row r="68" spans="2:8">
       <c r="B68" s="2">
-        <v>43895</v>
+        <v>43899</v>
       </c>
       <c r="C68">
-        <v>26121.3</v>
+        <v>23851</v>
       </c>
       <c r="D68">
-        <v>26121.3</v>
+        <v>23851</v>
       </c>
       <c r="E68">
-        <v>26121.3</v>
+        <v>23851</v>
       </c>
       <c r="F68">
-        <v>26121.3</v>
+        <v>23851</v>
       </c>
       <c r="G68">
-        <v>26121.3</v>
+        <v>23851</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -1970,22 +1970,22 @@
     </row>
     <row r="69" spans="2:8">
       <c r="B69" s="2">
-        <v>43896</v>
+        <v>43900</v>
       </c>
       <c r="C69">
-        <v>25864.8</v>
+        <v>25018.2</v>
       </c>
       <c r="D69">
-        <v>25864.8</v>
+        <v>25018.2</v>
       </c>
       <c r="E69">
-        <v>25864.8</v>
+        <v>25018.2</v>
       </c>
       <c r="F69">
-        <v>25864.8</v>
+        <v>25018.2</v>
       </c>
       <c r="G69">
-        <v>25864.8</v>
+        <v>25018.2</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -1993,22 +1993,22 @@
     </row>
     <row r="70" spans="2:8">
       <c r="B70" s="2">
-        <v>43899</v>
+        <v>43901</v>
       </c>
       <c r="C70">
-        <v>23851</v>
+        <v>23553.2</v>
       </c>
       <c r="D70">
-        <v>23851</v>
+        <v>23553.2</v>
       </c>
       <c r="E70">
-        <v>23851</v>
+        <v>23553.2</v>
       </c>
       <c r="F70">
-        <v>23851</v>
+        <v>23553.2</v>
       </c>
       <c r="G70">
-        <v>23851</v>
+        <v>23553.2</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -2016,22 +2016,22 @@
     </row>
     <row r="71" spans="2:8">
       <c r="B71" s="2">
-        <v>43900</v>
+        <v>43902</v>
       </c>
       <c r="C71">
-        <v>25018.2</v>
+        <v>21200.6</v>
       </c>
       <c r="D71">
-        <v>25018.2</v>
+        <v>21200.6</v>
       </c>
       <c r="E71">
-        <v>25018.2</v>
+        <v>21200.6</v>
       </c>
       <c r="F71">
-        <v>25018.2</v>
+        <v>21200.6</v>
       </c>
       <c r="G71">
-        <v>25018.2</v>
+        <v>21200.6</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -2039,22 +2039,22 @@
     </row>
     <row r="72" spans="2:8">
       <c r="B72" s="2">
-        <v>43901</v>
+        <v>43903</v>
       </c>
       <c r="C72">
-        <v>23553.2</v>
+        <v>23185.6</v>
       </c>
       <c r="D72">
-        <v>23553.2</v>
+        <v>23185.6</v>
       </c>
       <c r="E72">
-        <v>23553.2</v>
+        <v>23185.6</v>
       </c>
       <c r="F72">
-        <v>23553.2</v>
+        <v>23185.6</v>
       </c>
       <c r="G72">
-        <v>23553.2</v>
+        <v>23185.6</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -2062,22 +2062,22 @@
     </row>
     <row r="73" spans="2:8">
       <c r="B73" s="2">
-        <v>43902</v>
+        <v>43906</v>
       </c>
       <c r="C73">
-        <v>21200.6</v>
+        <v>20188.5</v>
       </c>
       <c r="D73">
-        <v>21200.6</v>
+        <v>20188.5</v>
       </c>
       <c r="E73">
-        <v>21200.6</v>
+        <v>20188.5</v>
       </c>
       <c r="F73">
-        <v>21200.6</v>
+        <v>20188.5</v>
       </c>
       <c r="G73">
-        <v>21200.6</v>
+        <v>20188.5</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -2085,22 +2085,22 @@
     </row>
     <row r="74" spans="2:8">
       <c r="B74" s="2">
-        <v>43903</v>
+        <v>43907</v>
       </c>
       <c r="C74">
-        <v>23185.6</v>
+        <v>21237.4</v>
       </c>
       <c r="D74">
-        <v>23185.6</v>
+        <v>21237.4</v>
       </c>
       <c r="E74">
-        <v>23185.6</v>
+        <v>21237.4</v>
       </c>
       <c r="F74">
-        <v>23185.6</v>
+        <v>21237.4</v>
       </c>
       <c r="G74">
-        <v>23185.6</v>
+        <v>21237.4</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -2108,22 +2108,22 @@
     </row>
     <row r="75" spans="2:8">
       <c r="B75" s="2">
-        <v>43906</v>
+        <v>43908</v>
       </c>
       <c r="C75">
-        <v>20188.5</v>
+        <v>19898.9</v>
       </c>
       <c r="D75">
-        <v>20188.5</v>
+        <v>19898.9</v>
       </c>
       <c r="E75">
-        <v>20188.5</v>
+        <v>19898.9</v>
       </c>
       <c r="F75">
-        <v>20188.5</v>
+        <v>19898.9</v>
       </c>
       <c r="G75">
-        <v>20188.5</v>
+        <v>19898.9</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -2131,22 +2131,22 @@
     </row>
     <row r="76" spans="2:8">
       <c r="B76" s="2">
-        <v>43907</v>
+        <v>43909</v>
       </c>
       <c r="C76">
-        <v>21237.4</v>
+        <v>20087.2</v>
       </c>
       <c r="D76">
-        <v>21237.4</v>
+        <v>20087.2</v>
       </c>
       <c r="E76">
-        <v>21237.4</v>
+        <v>20087.2</v>
       </c>
       <c r="F76">
-        <v>21237.4</v>
+        <v>20087.2</v>
       </c>
       <c r="G76">
-        <v>21237.4</v>
+        <v>20087.2</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -2154,22 +2154,22 @@
     </row>
     <row r="77" spans="2:8">
       <c r="B77" s="2">
-        <v>43908</v>
+        <v>43910</v>
       </c>
       <c r="C77">
-        <v>19898.9</v>
+        <v>19174</v>
       </c>
       <c r="D77">
-        <v>19898.9</v>
+        <v>19174</v>
       </c>
       <c r="E77">
-        <v>19898.9</v>
+        <v>19174</v>
       </c>
       <c r="F77">
-        <v>19898.9</v>
+        <v>19174</v>
       </c>
       <c r="G77">
-        <v>19898.9</v>
+        <v>19174</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -2177,22 +2177,22 @@
     </row>
     <row r="78" spans="2:8">
       <c r="B78" s="2">
-        <v>43909</v>
+        <v>43913</v>
       </c>
       <c r="C78">
-        <v>20087.2</v>
+        <v>18591.9</v>
       </c>
       <c r="D78">
-        <v>20087.2</v>
+        <v>18591.9</v>
       </c>
       <c r="E78">
-        <v>20087.2</v>
+        <v>18591.9</v>
       </c>
       <c r="F78">
-        <v>20087.2</v>
+        <v>18591.9</v>
       </c>
       <c r="G78">
-        <v>20087.2</v>
+        <v>18591.9</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -2200,22 +2200,22 @@
     </row>
     <row r="79" spans="2:8">
       <c r="B79" s="2">
-        <v>43910</v>
+        <v>43914</v>
       </c>
       <c r="C79">
-        <v>19174</v>
+        <v>20704.9</v>
       </c>
       <c r="D79">
-        <v>19174</v>
+        <v>20704.9</v>
       </c>
       <c r="E79">
-        <v>19174</v>
+        <v>20704.9</v>
       </c>
       <c r="F79">
-        <v>19174</v>
+        <v>20704.9</v>
       </c>
       <c r="G79">
-        <v>19174</v>
+        <v>20704.9</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -2223,22 +2223,22 @@
     </row>
     <row r="80" spans="2:8">
       <c r="B80" s="2">
-        <v>43913</v>
+        <v>43915</v>
       </c>
       <c r="C80">
-        <v>18591.9</v>
+        <v>21200.6</v>
       </c>
       <c r="D80">
-        <v>18591.9</v>
+        <v>21200.6</v>
       </c>
       <c r="E80">
-        <v>18591.9</v>
+        <v>21200.6</v>
       </c>
       <c r="F80">
-        <v>18591.9</v>
+        <v>21200.6</v>
       </c>
       <c r="G80">
-        <v>18591.9</v>
+        <v>21200.6</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -2246,22 +2246,22 @@
     </row>
     <row r="81" spans="2:8">
       <c r="B81" s="2">
-        <v>43914</v>
+        <v>43916</v>
       </c>
       <c r="C81">
-        <v>20704.9</v>
+        <v>22552.2</v>
       </c>
       <c r="D81">
-        <v>20704.9</v>
+        <v>22552.2</v>
       </c>
       <c r="E81">
-        <v>20704.9</v>
+        <v>22552.2</v>
       </c>
       <c r="F81">
-        <v>20704.9</v>
+        <v>22552.2</v>
       </c>
       <c r="G81">
-        <v>20704.9</v>
+        <v>22552.2</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -2269,22 +2269,22 @@
     </row>
     <row r="82" spans="2:8">
       <c r="B82" s="2">
-        <v>43915</v>
+        <v>43917</v>
       </c>
       <c r="C82">
-        <v>21200.6</v>
+        <v>21636.8</v>
       </c>
       <c r="D82">
-        <v>21200.6</v>
+        <v>21636.8</v>
       </c>
       <c r="E82">
-        <v>21200.6</v>
+        <v>21636.8</v>
       </c>
       <c r="F82">
-        <v>21200.6</v>
+        <v>21636.8</v>
       </c>
       <c r="G82">
-        <v>21200.6</v>
+        <v>21636.8</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -2292,22 +2292,22 @@
     </row>
     <row r="83" spans="2:8">
       <c r="B83" s="2">
-        <v>43916</v>
+        <v>43920</v>
       </c>
       <c r="C83">
-        <v>22552.2</v>
+        <v>22327.5</v>
       </c>
       <c r="D83">
-        <v>22552.2</v>
+        <v>22327.5</v>
       </c>
       <c r="E83">
-        <v>22552.2</v>
+        <v>22327.5</v>
       </c>
       <c r="F83">
-        <v>22552.2</v>
+        <v>22327.5</v>
       </c>
       <c r="G83">
-        <v>22552.2</v>
+        <v>22327.5</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -2315,22 +2315,22 @@
     </row>
     <row r="84" spans="2:8">
       <c r="B84" s="2">
-        <v>43917</v>
+        <v>43921</v>
       </c>
       <c r="C84">
-        <v>21636.8</v>
+        <v>21917.2</v>
       </c>
       <c r="D84">
-        <v>21636.8</v>
+        <v>21917.2</v>
       </c>
       <c r="E84">
-        <v>21636.8</v>
+        <v>21917.2</v>
       </c>
       <c r="F84">
-        <v>21636.8</v>
+        <v>21917.2</v>
       </c>
       <c r="G84">
-        <v>21636.8</v>
+        <v>21917.2</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -2338,22 +2338,22 @@
     </row>
     <row r="85" spans="2:8">
       <c r="B85" s="2">
-        <v>43920</v>
+        <v>43922</v>
       </c>
       <c r="C85">
-        <v>22327.5</v>
+        <v>20943.5</v>
       </c>
       <c r="D85">
-        <v>22327.5</v>
+        <v>20943.5</v>
       </c>
       <c r="E85">
-        <v>22327.5</v>
+        <v>20943.5</v>
       </c>
       <c r="F85">
-        <v>22327.5</v>
+        <v>20943.5</v>
       </c>
       <c r="G85">
-        <v>22327.5</v>
+        <v>20943.5</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -2361,22 +2361,22 @@
     </row>
     <row r="86" spans="2:8">
       <c r="B86" s="2">
-        <v>43921</v>
+        <v>43923</v>
       </c>
       <c r="C86">
-        <v>21917.2</v>
+        <v>21413.4</v>
       </c>
       <c r="D86">
-        <v>21917.2</v>
+        <v>21413.4</v>
       </c>
       <c r="E86">
-        <v>21917.2</v>
+        <v>21413.4</v>
       </c>
       <c r="F86">
-        <v>21917.2</v>
+        <v>21413.4</v>
       </c>
       <c r="G86">
-        <v>21917.2</v>
+        <v>21413.4</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -2384,22 +2384,22 @@
     </row>
     <row r="87" spans="2:8">
       <c r="B87" s="2">
-        <v>43922</v>
+        <v>43924</v>
       </c>
       <c r="C87">
-        <v>20943.5</v>
+        <v>21052.5</v>
       </c>
       <c r="D87">
-        <v>20943.5</v>
+        <v>21052.5</v>
       </c>
       <c r="E87">
-        <v>20943.5</v>
+        <v>21052.5</v>
       </c>
       <c r="F87">
-        <v>20943.5</v>
+        <v>21052.5</v>
       </c>
       <c r="G87">
-        <v>20943.5</v>
+        <v>21052.5</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -2407,22 +2407,22 @@
     </row>
     <row r="88" spans="2:8">
       <c r="B88" s="2">
-        <v>43923</v>
+        <v>43927</v>
       </c>
       <c r="C88">
-        <v>21413.4</v>
+        <v>22680</v>
       </c>
       <c r="D88">
-        <v>21413.4</v>
+        <v>22680</v>
       </c>
       <c r="E88">
-        <v>21413.4</v>
+        <v>22680</v>
       </c>
       <c r="F88">
-        <v>21413.4</v>
+        <v>22680</v>
       </c>
       <c r="G88">
-        <v>21413.4</v>
+        <v>22680</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -2430,22 +2430,22 @@
     </row>
     <row r="89" spans="2:8">
       <c r="B89" s="2">
-        <v>43924</v>
+        <v>43928</v>
       </c>
       <c r="C89">
-        <v>21052.5</v>
+        <v>22653.9</v>
       </c>
       <c r="D89">
-        <v>21052.5</v>
+        <v>22653.9</v>
       </c>
       <c r="E89">
-        <v>21052.5</v>
+        <v>22653.9</v>
       </c>
       <c r="F89">
-        <v>21052.5</v>
+        <v>22653.9</v>
       </c>
       <c r="G89">
-        <v>21052.5</v>
+        <v>22653.9</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -2453,22 +2453,22 @@
     </row>
     <row r="90" spans="2:8">
       <c r="B90" s="2">
-        <v>43927</v>
+        <v>43929</v>
       </c>
       <c r="C90">
-        <v>22680</v>
+        <v>23433.6</v>
       </c>
       <c r="D90">
-        <v>22680</v>
+        <v>23433.6</v>
       </c>
       <c r="E90">
-        <v>22680</v>
+        <v>23433.6</v>
       </c>
       <c r="F90">
-        <v>22680</v>
+        <v>23433.6</v>
       </c>
       <c r="G90">
-        <v>22680</v>
+        <v>23433.6</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -2476,22 +2476,22 @@
     </row>
     <row r="91" spans="2:8">
       <c r="B91" s="2">
-        <v>43928</v>
+        <v>43930</v>
       </c>
       <c r="C91">
-        <v>22653.9</v>
+        <v>23719.4</v>
       </c>
       <c r="D91">
-        <v>22653.9</v>
+        <v>23719.4</v>
       </c>
       <c r="E91">
-        <v>22653.9</v>
+        <v>23719.4</v>
       </c>
       <c r="F91">
-        <v>22653.9</v>
+        <v>23719.4</v>
       </c>
       <c r="G91">
-        <v>22653.9</v>
+        <v>23719.4</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -2499,22 +2499,22 @@
     </row>
     <row r="92" spans="2:8">
       <c r="B92" s="2">
-        <v>43929</v>
+        <v>43934</v>
       </c>
       <c r="C92">
-        <v>23433.6</v>
+        <v>23390.8</v>
       </c>
       <c r="D92">
-        <v>23433.6</v>
+        <v>23390.8</v>
       </c>
       <c r="E92">
-        <v>23433.6</v>
+        <v>23390.8</v>
       </c>
       <c r="F92">
-        <v>23433.6</v>
+        <v>23390.8</v>
       </c>
       <c r="G92">
-        <v>23433.6</v>
+        <v>23390.8</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -2522,22 +2522,22 @@
     </row>
     <row r="93" spans="2:8">
       <c r="B93" s="2">
-        <v>43930</v>
+        <v>43935</v>
       </c>
       <c r="C93">
-        <v>23719.4</v>
+        <v>23949.8</v>
       </c>
       <c r="D93">
-        <v>23719.4</v>
+        <v>23949.8</v>
       </c>
       <c r="E93">
-        <v>23719.4</v>
+        <v>23949.8</v>
       </c>
       <c r="F93">
-        <v>23719.4</v>
+        <v>23949.8</v>
       </c>
       <c r="G93">
-        <v>23719.4</v>
+        <v>23949.8</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -2545,22 +2545,22 @@
     </row>
     <row r="94" spans="2:8">
       <c r="B94" s="2">
-        <v>43934</v>
+        <v>43936</v>
       </c>
       <c r="C94">
-        <v>23390.8</v>
+        <v>23504.3</v>
       </c>
       <c r="D94">
-        <v>23390.8</v>
+        <v>23504.3</v>
       </c>
       <c r="E94">
-        <v>23390.8</v>
+        <v>23504.3</v>
       </c>
       <c r="F94">
-        <v>23390.8</v>
+        <v>23504.3</v>
       </c>
       <c r="G94">
-        <v>23390.8</v>
+        <v>23504.3</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -2568,22 +2568,22 @@
     </row>
     <row r="95" spans="2:8">
       <c r="B95" s="2">
-        <v>43935</v>
+        <v>43937</v>
       </c>
       <c r="C95">
-        <v>23949.8</v>
+        <v>23537.7</v>
       </c>
       <c r="D95">
-        <v>23949.8</v>
+        <v>23537.7</v>
       </c>
       <c r="E95">
-        <v>23949.8</v>
+        <v>23537.7</v>
       </c>
       <c r="F95">
-        <v>23949.8</v>
+        <v>23537.7</v>
       </c>
       <c r="G95">
-        <v>23949.8</v>
+        <v>23537.7</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -2591,47 +2591,24 @@
     </row>
     <row r="96" spans="2:8">
       <c r="B96" s="2">
-        <v>43936</v>
+        <v>43938</v>
       </c>
       <c r="C96">
-        <v>23504.3</v>
+        <v>24242.5</v>
       </c>
       <c r="D96">
-        <v>23504.3</v>
+        <v>24242.5</v>
       </c>
       <c r="E96">
-        <v>23504.3</v>
+        <v>24242.5</v>
       </c>
       <c r="F96">
-        <v>23504.3</v>
+        <v>24242.5</v>
       </c>
       <c r="G96">
-        <v>23504.3</v>
+        <v>24242.5</v>
       </c>
       <c r="H96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8">
-      <c r="B97" s="2">
-        <v>43937</v>
-      </c>
-      <c r="C97">
-        <v>23537.7</v>
-      </c>
-      <c r="D97">
-        <v>23537.7</v>
-      </c>
-      <c r="E97">
-        <v>23537.7</v>
-      </c>
-      <c r="F97">
-        <v>23537.7</v>
-      </c>
-      <c r="G97">
-        <v>23537.7</v>
-      </c>
-      <c r="H97">
         <v>0</v>
       </c>
     </row>

</xml_diff>